<commit_message>
Fixed issue with wrong WF Path on MD
</commit_message>
<xml_diff>
--- a/Cmf.Custom.IoT/OmegaPlasma/MasterData/OmegaPlasma.xlsx
+++ b/Cmf.Custom.IoT/OmegaPlasma/MasterData/OmegaPlasma.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CMF\Projects\AMSOSRAM\Cmf.Custom.IoT\OmegaPlasma\MasterData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gits\AMSOSRAM\Cmf.Custom.IoT\OmegaPlasma\MasterData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF767BD-C7BA-459F-8364-2F42D74544DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8D8E0A-054A-409B-8602-A4B65D4C82A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="23" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11235" firstSheet="23" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="2" r:id="rId1"/>
@@ -2626,7 +2626,7 @@
     <t>ReadyToLoad_01_EventReceived</t>
   </si>
   <si>
-    <t>OmegaPlasma\ReadyToLoad_01_EventReceived</t>
+    <t>OmegaPlasma\ReadyToLoad_01_EventReceived.json</t>
   </si>
 </sst>
 </file>
@@ -3017,14 +3017,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -3060,7 +3060,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -3110,7 +3110,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -3180,7 +3180,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
@@ -3205,7 +3205,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>40</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>42</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -3244,7 +3244,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>52</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>55</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>60</v>
       </c>
@@ -3308,7 +3308,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>62</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>65</v>
       </c>
@@ -3336,7 +3336,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>68</v>
       </c>
@@ -3350,7 +3350,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>71</v>
       </c>
@@ -3364,7 +3364,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>74</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>76</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>79</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>82</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>83</v>
       </c>
@@ -3419,7 +3419,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>84</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>87</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>90</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>93</v>
       </c>
@@ -3475,7 +3475,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>97</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>100</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>103</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>106</v>
       </c>
@@ -3528,7 +3528,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>108</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>111</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>114</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>117</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>120</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>123</v>
       </c>
@@ -3609,7 +3609,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>125</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>127</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>130</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>133</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>136</v>
       </c>
@@ -3670,7 +3670,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>138</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>141</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>143</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>146</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>149</v>
       </c>
@@ -3734,7 +3734,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>151</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>154</v>
       </c>
@@ -3762,7 +3762,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>157</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>159</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>162</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>165</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>168</v>
       </c>
@@ -3823,7 +3823,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>170</v>
       </c>
@@ -3837,7 +3837,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>173</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>176</v>
       </c>
@@ -3865,7 +3865,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>179</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>181</v>
       </c>
@@ -3890,7 +3890,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>184</v>
       </c>
@@ -3904,7 +3904,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>187</v>
       </c>
@@ -3915,7 +3915,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>189</v>
       </c>
@@ -3929,7 +3929,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>192</v>
       </c>
@@ -3943,7 +3943,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>195</v>
       </c>
@@ -3957,7 +3957,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>198</v>
       </c>
@@ -3968,7 +3968,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>200</v>
       </c>
@@ -3979,7 +3979,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>202</v>
       </c>
@@ -3990,7 +3990,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>204</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>207</v>
       </c>
@@ -4015,7 +4015,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>209</v>
       </c>
@@ -4026,7 +4026,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>211</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>214</v>
       </c>
@@ -4054,7 +4054,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>218</v>
       </c>
@@ -4065,7 +4065,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>220</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>222</v>
       </c>
@@ -4090,7 +4090,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>226</v>
       </c>
@@ -4098,7 +4098,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>227</v>
       </c>
@@ -4106,7 +4106,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>228</v>
       </c>
@@ -4120,7 +4120,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>231</v>
       </c>
@@ -4134,7 +4134,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>234</v>
       </c>
@@ -4148,7 +4148,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>237</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>239</v>
       </c>
@@ -4173,7 +4173,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>242</v>
       </c>
@@ -4187,7 +4187,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>245</v>
       </c>
@@ -4201,7 +4201,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>248</v>
       </c>
@@ -4215,7 +4215,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>250</v>
       </c>
@@ -4229,7 +4229,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>252</v>
       </c>
@@ -4243,7 +4243,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>254</v>
       </c>
@@ -4254,7 +4254,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>256</v>
       </c>
@@ -4268,7 +4268,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>259</v>
       </c>
@@ -4292,17 +4292,17 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>423</v>
       </c>
@@ -4328,7 +4328,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>422</v>
       </c>
@@ -4345,7 +4345,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>422</v>
       </c>
@@ -4373,7 +4373,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -4385,7 +4385,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -4397,7 +4397,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -4409,7 +4409,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -4421,7 +4421,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -4433,7 +4433,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -4447,16 +4447,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>419</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>494</v>
       </c>
@@ -4503,17 +4503,17 @@
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>453</v>
       </c>
@@ -4533,7 +4533,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>494</v>
       </c>
@@ -4550,7 +4550,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>494</v>
       </c>
@@ -4567,7 +4567,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>494</v>
       </c>
@@ -4584,7 +4584,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>494</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>494</v>
       </c>
@@ -4618,7 +4618,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>494</v>
       </c>
@@ -4635,7 +4635,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>494</v>
       </c>
@@ -4652,7 +4652,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>494</v>
       </c>
@@ -4669,7 +4669,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>494</v>
       </c>
@@ -4686,7 +4686,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>494</v>
       </c>
@@ -4703,7 +4703,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>494</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>494</v>
       </c>
@@ -4737,7 +4737,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>494</v>
       </c>
@@ -4754,7 +4754,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>494</v>
       </c>
@@ -4771,7 +4771,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>494</v>
       </c>
@@ -4788,7 +4788,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>494</v>
       </c>
@@ -4805,7 +4805,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>494</v>
       </c>
@@ -4822,7 +4822,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>494</v>
       </c>
@@ -4839,7 +4839,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>494</v>
       </c>
@@ -4856,7 +4856,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>494</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>494</v>
       </c>
@@ -4890,7 +4890,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>494</v>
       </c>
@@ -4907,7 +4907,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>494</v>
       </c>
@@ -4924,7 +4924,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>494</v>
       </c>
@@ -4941,7 +4941,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>494</v>
       </c>
@@ -4958,7 +4958,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>494</v>
       </c>
@@ -4975,7 +4975,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>494</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>494</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>494</v>
       </c>
@@ -5026,7 +5026,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>494</v>
       </c>
@@ -5043,7 +5043,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>494</v>
       </c>
@@ -5060,7 +5060,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>494</v>
       </c>
@@ -5077,7 +5077,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>494</v>
       </c>
@@ -5094,7 +5094,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>494</v>
       </c>
@@ -5111,7 +5111,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>494</v>
       </c>
@@ -5128,7 +5128,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>494</v>
       </c>
@@ -5145,7 +5145,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>494</v>
       </c>
@@ -5162,7 +5162,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>494</v>
       </c>
@@ -5179,7 +5179,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>494</v>
       </c>
@@ -5196,7 +5196,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>494</v>
       </c>
@@ -5213,7 +5213,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>494</v>
       </c>
@@ -5230,7 +5230,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>494</v>
       </c>
@@ -5247,7 +5247,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>494</v>
       </c>
@@ -5264,7 +5264,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>494</v>
       </c>
@@ -5281,7 +5281,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>494</v>
       </c>
@@ -5298,7 +5298,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>494</v>
       </c>
@@ -5315,7 +5315,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>494</v>
       </c>
@@ -5332,7 +5332,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>494</v>
       </c>
@@ -5349,7 +5349,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>494</v>
       </c>
@@ -5366,7 +5366,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>494</v>
       </c>
@@ -5383,7 +5383,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>494</v>
       </c>
@@ -5400,7 +5400,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>494</v>
       </c>
@@ -5417,7 +5417,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>494</v>
       </c>
@@ -5434,7 +5434,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>494</v>
       </c>
@@ -5451,7 +5451,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>494</v>
       </c>
@@ -5468,7 +5468,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>494</v>
       </c>
@@ -5485,7 +5485,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>494</v>
       </c>
@@ -5502,7 +5502,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>494</v>
       </c>
@@ -5519,7 +5519,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>494</v>
       </c>
@@ -5536,7 +5536,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>494</v>
       </c>
@@ -5553,7 +5553,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>494</v>
       </c>
@@ -5570,7 +5570,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>494</v>
       </c>
@@ -5587,7 +5587,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>494</v>
       </c>
@@ -5604,7 +5604,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>494</v>
       </c>
@@ -5621,7 +5621,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>494</v>
       </c>
@@ -5638,7 +5638,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>494</v>
       </c>
@@ -5655,7 +5655,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>494</v>
       </c>
@@ -5672,7 +5672,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>494</v>
       </c>
@@ -5689,7 +5689,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>494</v>
       </c>
@@ -5706,7 +5706,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>494</v>
       </c>
@@ -5723,7 +5723,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>494</v>
       </c>
@@ -5740,7 +5740,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>494</v>
       </c>
@@ -5757,7 +5757,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>494</v>
       </c>
@@ -5774,7 +5774,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>494</v>
       </c>
@@ -5791,7 +5791,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>494</v>
       </c>
@@ -5808,7 +5808,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>494</v>
       </c>
@@ -5825,7 +5825,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>494</v>
       </c>
@@ -5842,7 +5842,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>494</v>
       </c>
@@ -5859,7 +5859,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>494</v>
       </c>
@@ -5876,7 +5876,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>494</v>
       </c>
@@ -5893,7 +5893,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>494</v>
       </c>
@@ -5910,7 +5910,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>494</v>
       </c>
@@ -5927,7 +5927,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>494</v>
       </c>
@@ -5944,7 +5944,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>494</v>
       </c>
@@ -5961,7 +5961,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>494</v>
       </c>
@@ -5978,7 +5978,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>494</v>
       </c>
@@ -5995,7 +5995,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>494</v>
       </c>
@@ -6037,16 +6037,16 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>453</v>
       </c>
@@ -6063,7 +6063,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>494</v>
       </c>
@@ -6080,7 +6080,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>494</v>
       </c>
@@ -6097,7 +6097,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>494</v>
       </c>
@@ -6114,7 +6114,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>494</v>
       </c>
@@ -6131,7 +6131,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>494</v>
       </c>
@@ -6148,7 +6148,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>494</v>
       </c>
@@ -6165,7 +6165,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>494</v>
       </c>
@@ -6182,7 +6182,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>494</v>
       </c>
@@ -6199,7 +6199,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>494</v>
       </c>
@@ -6216,7 +6216,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>494</v>
       </c>
@@ -6233,7 +6233,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>494</v>
       </c>
@@ -6250,7 +6250,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>494</v>
       </c>
@@ -6267,7 +6267,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>494</v>
       </c>
@@ -6284,7 +6284,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>494</v>
       </c>
@@ -6301,7 +6301,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>494</v>
       </c>
@@ -6318,7 +6318,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>494</v>
       </c>
@@ -6335,7 +6335,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>494</v>
       </c>
@@ -6352,7 +6352,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>494</v>
       </c>
@@ -6369,7 +6369,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>494</v>
       </c>
@@ -6386,7 +6386,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>494</v>
       </c>
@@ -6403,7 +6403,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>494</v>
       </c>
@@ -6420,7 +6420,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>494</v>
       </c>
@@ -6437,7 +6437,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>494</v>
       </c>
@@ -6454,7 +6454,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>494</v>
       </c>
@@ -6471,7 +6471,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>494</v>
       </c>
@@ -6488,7 +6488,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>494</v>
       </c>
@@ -6505,7 +6505,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>494</v>
       </c>
@@ -6522,7 +6522,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>494</v>
       </c>
@@ -6539,7 +6539,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>494</v>
       </c>
@@ -6556,7 +6556,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>494</v>
       </c>
@@ -6573,7 +6573,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>494</v>
       </c>
@@ -6590,7 +6590,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>494</v>
       </c>
@@ -6607,7 +6607,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>494</v>
       </c>
@@ -6624,7 +6624,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>494</v>
       </c>
@@ -6641,7 +6641,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>494</v>
       </c>
@@ -6658,7 +6658,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>494</v>
       </c>
@@ -6675,7 +6675,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>494</v>
       </c>
@@ -6692,7 +6692,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>494</v>
       </c>
@@ -6709,7 +6709,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>494</v>
       </c>
@@ -6738,9 +6738,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>262</v>
       </c>
@@ -6754,7 +6754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>265</v>
       </c>
@@ -6768,7 +6768,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>265</v>
       </c>
@@ -6782,7 +6782,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>265</v>
       </c>
@@ -6796,7 +6796,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>38</v>
       </c>
@@ -6810,7 +6810,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>40</v>
       </c>
@@ -6824,7 +6824,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>74</v>
       </c>
@@ -6838,7 +6838,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>282</v>
       </c>
@@ -6852,7 +6852,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>141</v>
       </c>
@@ -6866,7 +6866,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>289</v>
       </c>
@@ -6880,7 +6880,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>289</v>
       </c>
@@ -6894,7 +6894,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>289</v>
       </c>
@@ -6908,7 +6908,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>299</v>
       </c>
@@ -6922,7 +6922,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>168</v>
       </c>
@@ -6936,7 +6936,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>305</v>
       </c>
@@ -6950,7 +6950,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>187</v>
       </c>
@@ -6964,7 +6964,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>312</v>
       </c>
@@ -6978,7 +6978,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>312</v>
       </c>
@@ -6992,7 +6992,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>200</v>
       </c>
@@ -7019,20 +7019,20 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="157" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>453</v>
       </c>
@@ -7061,7 +7061,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>494</v>
       </c>
@@ -7090,7 +7090,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>494</v>
       </c>
@@ -7119,7 +7119,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>494</v>
       </c>
@@ -7148,7 +7148,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>494</v>
       </c>
@@ -7177,7 +7177,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>494</v>
       </c>
@@ -7206,7 +7206,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>494</v>
       </c>
@@ -7235,7 +7235,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>494</v>
       </c>
@@ -7264,7 +7264,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>494</v>
       </c>
@@ -7293,7 +7293,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>494</v>
       </c>
@@ -7322,7 +7322,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>494</v>
       </c>
@@ -7351,7 +7351,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>494</v>
       </c>
@@ -7380,7 +7380,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>494</v>
       </c>
@@ -7409,7 +7409,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>494</v>
       </c>
@@ -7438,7 +7438,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>494</v>
       </c>
@@ -7467,7 +7467,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>494</v>
       </c>
@@ -7496,7 +7496,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>494</v>
       </c>
@@ -7525,7 +7525,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>494</v>
       </c>
@@ -7554,7 +7554,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>494</v>
       </c>
@@ -7583,7 +7583,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>494</v>
       </c>
@@ -7612,7 +7612,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>494</v>
       </c>
@@ -7659,16 +7659,16 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>453</v>
       </c>
@@ -7685,7 +7685,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>494</v>
       </c>
@@ -7702,7 +7702,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>494</v>
       </c>
@@ -7719,7 +7719,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>494</v>
       </c>
@@ -7736,7 +7736,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>494</v>
       </c>
@@ -7753,7 +7753,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>494</v>
       </c>
@@ -7770,7 +7770,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>494</v>
       </c>
@@ -7787,7 +7787,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>494</v>
       </c>
@@ -7804,7 +7804,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>494</v>
       </c>
@@ -7821,7 +7821,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>494</v>
       </c>
@@ -7838,7 +7838,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>494</v>
       </c>
@@ -7855,7 +7855,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>494</v>
       </c>
@@ -7886,21 +7886,21 @@
       <selection activeCell="C9" sqref="B8:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>453</v>
       </c>
@@ -7932,7 +7932,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>494</v>
       </c>
@@ -7958,7 +7958,7 @@
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>494</v>
       </c>
@@ -7983,7 +7983,7 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>494</v>
       </c>
@@ -8007,7 +8007,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>494</v>
       </c>
@@ -8031,7 +8031,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>494</v>
       </c>
@@ -8055,7 +8055,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>494</v>
       </c>
@@ -8079,7 +8079,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>494</v>
       </c>
@@ -8103,7 +8103,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>494</v>
       </c>
@@ -8127,7 +8127,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>494</v>
       </c>
@@ -8151,7 +8151,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>494</v>
       </c>
@@ -8175,7 +8175,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>494</v>
       </c>
@@ -8199,7 +8199,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>494</v>
       </c>
@@ -8223,7 +8223,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>494</v>
       </c>
@@ -8261,18 +8261,18 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="168.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="168.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>419</v>
       </c>
@@ -8295,7 +8295,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>784</v>
       </c>
@@ -8331,15 +8331,15 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>451</v>
       </c>
@@ -8356,7 +8356,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>784</v>
       </c>
@@ -8373,7 +8373,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>784</v>
       </c>
@@ -8399,20 +8399,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="57.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="82.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="57.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="82.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>451</v>
       </c>
@@ -8432,7 +8432,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>784</v>
       </c>
@@ -8452,7 +8452,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>784</v>
       </c>
@@ -8472,7 +8472,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>784</v>
       </c>
@@ -8492,7 +8492,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>784</v>
       </c>
@@ -8512,7 +8512,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>784</v>
       </c>
@@ -8532,7 +8532,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>784</v>
       </c>
@@ -8552,7 +8552,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>784</v>
       </c>
@@ -8572,7 +8572,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>784</v>
       </c>
@@ -8592,7 +8592,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>784</v>
       </c>
@@ -8612,7 +8612,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>784</v>
       </c>
@@ -8632,7 +8632,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>784</v>
       </c>
@@ -8652,7 +8652,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>784</v>
       </c>
@@ -8672,7 +8672,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>784</v>
       </c>
@@ -8692,7 +8692,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>784</v>
       </c>
@@ -8712,7 +8712,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>784</v>
       </c>
@@ -8732,7 +8732,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>784</v>
       </c>
@@ -8752,7 +8752,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>784</v>
       </c>
@@ -8772,7 +8772,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>784</v>
       </c>
@@ -8792,7 +8792,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>784</v>
       </c>
@@ -8812,7 +8812,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>784</v>
       </c>
@@ -8832,7 +8832,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>784</v>
       </c>
@@ -8852,7 +8852,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>784</v>
       </c>
@@ -8872,7 +8872,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>784</v>
       </c>
@@ -8892,7 +8892,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>784</v>
       </c>
@@ -8912,7 +8912,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>784</v>
       </c>
@@ -8932,7 +8932,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>784</v>
       </c>
@@ -8952,7 +8952,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>784</v>
       </c>
@@ -8972,7 +8972,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>784</v>
       </c>
@@ -8992,7 +8992,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>784</v>
       </c>
@@ -9012,7 +9012,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>784</v>
       </c>
@@ -9032,7 +9032,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>784</v>
       </c>
@@ -9052,7 +9052,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>784</v>
       </c>
@@ -9084,7 +9084,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -9096,9 +9096,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>262</v>
       </c>
@@ -9106,7 +9106,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>265</v>
       </c>
@@ -9114,7 +9114,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>265</v>
       </c>
@@ -9122,7 +9122,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>283</v>
       </c>
@@ -9130,7 +9130,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>325</v>
       </c>
@@ -9138,7 +9138,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>327</v>
       </c>
@@ -9146,7 +9146,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>329</v>
       </c>
@@ -9165,9 +9165,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>330</v>
       </c>
@@ -9175,7 +9175,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>332</v>
       </c>
@@ -9183,7 +9183,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>254</v>
       </c>
@@ -9202,434 +9202,434 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>418</v>
       </c>
@@ -9645,7 +9645,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -9657,7 +9657,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -9671,15 +9671,15 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>419</v>
       </c>
@@ -9693,7 +9693,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>422</v>
       </c>
@@ -9714,17 +9714,17 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="52" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>423</v>
       </c>
@@ -9747,7 +9747,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>422</v>
       </c>
@@ -9767,7 +9767,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>422</v>
       </c>

</xml_diff>